<commit_message>
Finalize incl text runoff
</commit_message>
<xml_diff>
--- a/Outputs/appendix/a-tables.xlsx
+++ b/Outputs/appendix/a-tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbdaniels/GitHub/ssm-rhcp-2019/Outputs/appendix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7509E9-E980-6D4B-9D98-BB6CDFDB9996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F524B561-3475-054E-B3E5-461CD4E8008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="364">
   <si>
     <t>Andhra Pradesh</t>
   </si>
@@ -127,18 +129,6 @@
   </si>
   <si>
     <t>Adult primary education</t>
-  </si>
-  <si>
-    <t>Chattisgarh</t>
-  </si>
-  <si>
-    <t>Maharastra</t>
-  </si>
-  <si>
-    <t>Orissa</t>
-  </si>
-  <si>
-    <t>Tamilnadu</t>
   </si>
   <si>
     <t>Uttaranchal</t>
@@ -475,18 +465,9 @@
     <t>14.74</t>
   </si>
   <si>
-    <t>15.24</t>
-  </si>
-  <si>
-    <t>1.26</t>
-  </si>
-  <si>
     <t>21.18</t>
   </si>
   <si>
-    <t>24.97</t>
-  </si>
-  <si>
     <t>0.78</t>
   </si>
   <si>
@@ -496,9 +477,6 @@
     <t>26.39</t>
   </si>
   <si>
-    <t>26.66</t>
-  </si>
-  <si>
     <t>-1.14</t>
   </si>
   <si>
@@ -508,9 +486,6 @@
     <t>18.37</t>
   </si>
   <si>
-    <t>20.20</t>
-  </si>
-  <si>
     <t>0.10</t>
   </si>
   <si>
@@ -550,27 +525,18 @@
     <t>35.69</t>
   </si>
   <si>
-    <t>37.48</t>
-  </si>
-  <si>
     <t>-0.51</t>
   </si>
   <si>
     <t>23.33</t>
   </si>
   <si>
-    <t>24.26</t>
-  </si>
-  <si>
     <t>1.09</t>
   </si>
   <si>
     <t>29.36</t>
   </si>
   <si>
-    <t>27.04</t>
-  </si>
-  <si>
     <t>1.21</t>
   </si>
   <si>
@@ -583,12 +549,6 @@
     <t>-0.33</t>
   </si>
   <si>
-    <t>-0.32</t>
-  </si>
-  <si>
-    <t>38.07</t>
-  </si>
-  <si>
     <t>0.42</t>
   </si>
   <si>
@@ -598,15 +558,9 @@
     <t>36.79</t>
   </si>
   <si>
-    <t>38.23</t>
-  </si>
-  <si>
     <t>23.62</t>
   </si>
   <si>
-    <t>23.98</t>
-  </si>
-  <si>
     <t>-0.44</t>
   </si>
   <si>
@@ -616,51 +570,30 @@
     <t>38.38</t>
   </si>
   <si>
-    <t>39.26</t>
-  </si>
-  <si>
     <t>0.74</t>
   </si>
   <si>
     <t>19.65</t>
   </si>
   <si>
-    <t>19.86</t>
-  </si>
-  <si>
     <t>1.19</t>
   </si>
   <si>
-    <t>1.15</t>
-  </si>
-  <si>
     <t>23.83</t>
   </si>
   <si>
-    <t>24.09</t>
-  </si>
-  <si>
     <t>-1.11</t>
   </si>
   <si>
     <t>12.98</t>
   </si>
   <si>
-    <t>13.13</t>
-  </si>
-  <si>
     <t>-0.17</t>
   </si>
   <si>
-    <t>-0.19</t>
-  </si>
-  <si>
     <t>28.86</t>
   </si>
   <si>
-    <t>30.28</t>
-  </si>
-  <si>
     <t>0.02</t>
   </si>
   <si>
@@ -1130,6 +1063,72 @@
   </si>
   <si>
     <t>Panel C: Non-MBBS Providers</t>
+  </si>
+  <si>
+    <t>15.20</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>24.92</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>26.67</t>
+  </si>
+  <si>
+    <t>20.33</t>
+  </si>
+  <si>
+    <t>35.23</t>
+  </si>
+  <si>
+    <t>37.49</t>
+  </si>
+  <si>
+    <t>24.35</t>
+  </si>
+  <si>
+    <t>26.93</t>
+  </si>
+  <si>
+    <t>-0.31</t>
+  </si>
+  <si>
+    <t>38.19</t>
+  </si>
+  <si>
+    <t>38.20</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>23.95</t>
+  </si>
+  <si>
+    <t>39.27</t>
+  </si>
+  <si>
+    <t>19.78</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>24.10</t>
+  </si>
+  <si>
+    <t>13.08</t>
+  </si>
+  <si>
+    <t>-0.20</t>
+  </si>
+  <si>
+    <t>30.18</t>
   </si>
 </sst>
 </file>
@@ -1371,11 +1370,11 @@
     <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="37" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1397,6 +1396,20 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1417,20 +1430,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1525,6 +1524,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1568,9 +1570,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1608,6 +1607,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1657,22 +1675,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1682,6 +1695,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
@@ -1690,7 +1718,11 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1701,6 +1733,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1715,6 +1748,20 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1735,54 +1782,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1877,6 +1876,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1920,9 +1922,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1960,6 +1959,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2009,22 +2027,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2034,6 +2047,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
@@ -2042,7 +2070,11 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2053,6 +2085,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2067,6 +2100,20 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2087,54 +2134,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2229,6 +2228,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2272,9 +2274,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2312,6 +2311,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2361,22 +2379,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2386,6 +2399,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
@@ -2394,7 +2422,11 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2405,10 +2437,15 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2419,101 +2456,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2540,6 +2483,26 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2569,6 +2532,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2596,6 +2578,23 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2616,6 +2615,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2665,22 +2683,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2690,6 +2703,21 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
@@ -2698,7 +2726,11 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2709,115 +2741,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2906,6 +2832,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2932,6 +2875,26 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2961,6 +2924,25 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2988,6 +2970,23 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3008,6 +3007,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3057,22 +3075,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3082,40 +3095,26 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4093,70 +4092,70 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{34AA36A9-6B63-7249-A7A3-3B31342EA767}" name="Table16" displayName="Table16" ref="A3:G21" headerRowCount="0" headerRowDxfId="99" dataDxfId="98" totalsRowDxfId="97" headerRowBorderDxfId="95" tableBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{34AA36A9-6B63-7249-A7A3-3B31342EA767}" name="Table16" displayName="Table16" ref="A3:G21" headerRowCount="0" headerRowDxfId="99" dataDxfId="97" totalsRowDxfId="95" headerRowBorderDxfId="98" tableBorderDxfId="96">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{78A1AA99-864A-234E-8831-CF18A35739A7}" name="State" totalsRowLabel="Total" headerRowDxfId="93" dataDxfId="92" totalsRowDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{6B00846D-1A3F-1E44-85A8-2A0930FDA57B}" name="Monthly Patients per Public MBBS" headerRowDxfId="91" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{3F389B8E-7F27-994E-8CA0-6789FB794D84}" name="Average Monthly Public MBBS Salary" headerRowDxfId="89" dataDxfId="79" totalsRowDxfId="90" dataCellStyle="Currency"/>
-    <tableColumn id="2" xr3:uid="{6E37888A-6900-2A4C-97A8-B9E7AE5992B0}" name="Public Sector Patient Share" headerRowDxfId="88" dataDxfId="77" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{C75D2FFF-E6FF-5942-9904-E4B0C5AE7F4F}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="87" dataDxfId="78" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{F429F5B1-E6E5-B649-8A34-9245EA9D3182}" name="Average Private Non-MBBS Fee" headerRowDxfId="85" dataDxfId="84" totalsRowDxfId="86" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{EAE063E8-067A-D34F-9133-C68F236776D7}" name="Total Cost Per Patient" headerRowDxfId="82" dataDxfId="81" totalsRowDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{78A1AA99-864A-234E-8831-CF18A35739A7}" name="State" totalsRowLabel="Total" headerRowDxfId="94" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{6B00846D-1A3F-1E44-85A8-2A0930FDA57B}" name="Monthly Patients per Public MBBS" headerRowDxfId="91" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{3F389B8E-7F27-994E-8CA0-6789FB794D84}" name="Average Monthly Public MBBS Salary" headerRowDxfId="89" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{6E37888A-6900-2A4C-97A8-B9E7AE5992B0}" name="Public Sector Patient Share" headerRowDxfId="86" dataDxfId="85" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{C75D2FFF-E6FF-5942-9904-E4B0C5AE7F4F}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="84" dataDxfId="83" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{F429F5B1-E6E5-B649-8A34-9245EA9D3182}" name="Average Private Non-MBBS Fee" headerRowDxfId="82" dataDxfId="81" totalsRowDxfId="80" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{EAE063E8-067A-D34F-9133-C68F236776D7}" name="Total Cost Per Patient" headerRowDxfId="79" dataDxfId="78" totalsRowDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CEAE793E-47CA-E440-BA61-5C1EBB362213}" name="Table167" displayName="Table167" ref="A3:E21" headerRowCount="0" headerRowDxfId="76" dataDxfId="75" totalsRowDxfId="74" headerRowBorderDxfId="72" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CEAE793E-47CA-E440-BA61-5C1EBB362213}" name="Table167" displayName="Table167" ref="A3:E21" headerRowCount="0" headerRowDxfId="76" dataDxfId="74" totalsRowDxfId="72" headerRowBorderDxfId="75" tableBorderDxfId="73">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7CFA6A10-738A-684B-B183-1605F0F0CC07}" name="State" totalsRowLabel="Total" headerRowDxfId="70" dataDxfId="69" totalsRowDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{98279225-485A-C342-AB39-FEED2D6C80A9}" name="Monthly Patients per Public MBBS" headerRowDxfId="68" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{13F3380D-52ED-8545-A2B2-FD1186D48D6D}" name="Average Monthly Public MBBS Salary" headerRowDxfId="66" dataDxfId="62" totalsRowDxfId="67" dataCellStyle="Currency"/>
-    <tableColumn id="2" xr3:uid="{183C9F79-8558-A143-92B7-3827F7E12B05}" name="Public Sector Patient Share" headerRowDxfId="65" dataDxfId="61" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{5FBB5A9D-2BDC-4344-858C-6CC6EF70A246}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="64" dataDxfId="60" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{7CFA6A10-738A-684B-B183-1605F0F0CC07}" name="State" totalsRowLabel="Total" headerRowDxfId="71" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{98279225-485A-C342-AB39-FEED2D6C80A9}" name="Monthly Patients per Public MBBS" headerRowDxfId="68" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{13F3380D-52ED-8545-A2B2-FD1186D48D6D}" name="Average Monthly Public MBBS Salary" headerRowDxfId="66" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{183C9F79-8558-A143-92B7-3827F7E12B05}" name="Public Sector Patient Share" headerRowDxfId="63" dataDxfId="62" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{5FBB5A9D-2BDC-4344-858C-6CC6EF70A246}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="61" dataDxfId="60" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2910E91A-230C-194A-A035-D5870DA5AA27}" name="Table1678" displayName="Table1678" ref="A5:F18" headerRowCount="0" headerRowDxfId="59" dataDxfId="58" totalsRowDxfId="57" headerRowBorderDxfId="55" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2910E91A-230C-194A-A035-D5870DA5AA27}" name="Table1678" displayName="Table1678" ref="A5:F18" headerRowCount="0" headerRowDxfId="59" dataDxfId="57" totalsRowDxfId="55" headerRowBorderDxfId="58" tableBorderDxfId="56">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C53374B4-D126-0043-84E2-37BC26645E4B}" name="State" totalsRowLabel="Total" headerRowDxfId="53" dataDxfId="52" totalsRowDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{C53374B4-D126-0043-84E2-37BC26645E4B}" name="State" totalsRowLabel="Total" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52"/>
     <tableColumn id="6" xr3:uid="{4DED8158-C60E-3E40-8E38-29E26402987C}" name="Monthly Patients per Public MBBS" headerRowDxfId="51" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{4E5F7662-8FA0-3C45-8FFE-98461D650BA8}" name="Average Monthly Public MBBS Salary" headerRowDxfId="48" dataDxfId="47" totalsRowDxfId="49" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{4E5F7662-8FA0-3C45-8FFE-98461D650BA8}" name="Average Monthly Public MBBS Salary" headerRowDxfId="49" dataDxfId="48" totalsRowDxfId="47" dataCellStyle="Currency"/>
     <tableColumn id="2" xr3:uid="{281B6B53-CE81-F14D-A01F-1F57F8E9048C}" name="Public Sector Patient Share" headerRowDxfId="46" dataDxfId="45" dataCellStyle="Percent"/>
     <tableColumn id="8" xr3:uid="{FFF69F03-1A58-E74A-B92E-B00AEBAA72EF}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="44" dataDxfId="43" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{B4FD0CA5-79DE-434E-854A-2E3382531020}" name="Column1" headerRowDxfId="41" dataDxfId="42" totalsRowDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{B4FD0CA5-79DE-434E-854A-2E3382531020}" name="Column1" headerRowDxfId="42" dataDxfId="41" totalsRowDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C94F64A-6CC2-0546-ACF2-ED0D7EB602AB}" name="Table16789" displayName="Table16789" ref="A19:F29" headerRowCount="0" headerRowDxfId="39" dataDxfId="38" totalsRowDxfId="37" headerRowBorderDxfId="35" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C94F64A-6CC2-0546-ACF2-ED0D7EB602AB}" name="Table16789" displayName="Table16789" ref="A19:F29" headerRowCount="0" headerRowDxfId="39" dataDxfId="37" totalsRowDxfId="35" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9733455-32D0-D140-9A72-58D973E56438}" name="State" totalsRowLabel="Total" headerRowDxfId="33" dataDxfId="32" totalsRowDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{C9733455-32D0-D140-9A72-58D973E56438}" name="State" totalsRowLabel="Total" headerRowDxfId="34" dataDxfId="33" totalsRowDxfId="32"/>
     <tableColumn id="6" xr3:uid="{16DEFA58-86DD-BD4A-96C8-9624D32A2E46}" name="Monthly Patients per Public MBBS" headerRowDxfId="31" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{1B5A8F61-5D91-B244-9ADB-B864AC3991E3}" name="Average Monthly Public MBBS Salary" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="29" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{1B5A8F61-5D91-B244-9ADB-B864AC3991E3}" name="Average Monthly Public MBBS Salary" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Currency"/>
     <tableColumn id="2" xr3:uid="{8D6986E1-53B8-6141-9291-0A820F940C7A}" name="Public Sector Patient Share" headerRowDxfId="26" dataDxfId="25" dataCellStyle="Percent"/>
     <tableColumn id="8" xr3:uid="{F8F188E6-2380-C54B-A98D-EFA5E88FAEE3}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="24" dataDxfId="23" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{2825A4C3-6994-0647-90F5-153C2765B100}" name="Column1" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{2825A4C3-6994-0647-90F5-153C2765B100}" name="Column1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{080A84F8-2812-3C4B-9303-26A0684DCC61}" name="Table1678910" displayName="Table1678910" ref="A30:F39" headerRowCount="0" headerRowDxfId="19" dataDxfId="18" totalsRowDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{080A84F8-2812-3C4B-9303-26A0684DCC61}" name="Table1678910" displayName="Table1678910" ref="A30:F39" headerRowCount="0" headerRowDxfId="19" dataDxfId="17" totalsRowDxfId="15" headerRowBorderDxfId="18" tableBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{44B5AABC-8CAF-924D-B161-DCB573EA2D00}" name="State" totalsRowLabel="Total" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{44B5AABC-8CAF-924D-B161-DCB573EA2D00}" name="State" totalsRowLabel="Total" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="6" xr3:uid="{B2745CCF-2FDD-A847-B2AE-3514435E5230}" name="Monthly Patients per Public MBBS" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{3B3B83FD-0E24-D94D-880A-A30252CDC9A7}" name="Average Monthly Public MBBS Salary" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{3B3B83FD-0E24-D94D-880A-A30252CDC9A7}" name="Average Monthly Public MBBS Salary" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Currency"/>
     <tableColumn id="2" xr3:uid="{FC0246CC-B611-EE42-A5DB-DADCD7C2D00F}" name="Public Sector Patient Share" headerRowDxfId="6" dataDxfId="5" dataCellStyle="Percent"/>
     <tableColumn id="8" xr3:uid="{47910624-1ABA-4F43-AB43-950B4C5CBA2C}" name="Average _x000a_Public Sector Patient Cost" headerRowDxfId="4" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{FEFA43B9-1CE4-1646-B3FD-19683A5A305D}" name="Column1" headerRowDxfId="1" dataDxfId="0" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{FEFA43B9-1CE4-1646-B3FD-19683A5A305D}" name="Column1" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4462,7 +4461,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:H21"/>
+      <selection sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4499,19 +4498,19 @@
     <row r="2" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>21</v>
@@ -4707,16 +4706,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6">
         <v>35</v>
@@ -4967,16 +4966,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F20" s="6">
         <v>12</v>
@@ -5028,7 +5027,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:J21"/>
+      <selection sqref="A1:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5192,7 +5191,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>0.21645020000000001</v>
@@ -5448,7 +5447,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3">
         <v>0.46250000000000002</v>
@@ -5480,7 +5479,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3">
         <v>0.2708333</v>
@@ -5576,7 +5575,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>0.41583330000000002</v>
@@ -5640,7 +5639,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3">
         <v>0.68485419999999997</v>
@@ -5716,7 +5715,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5749,24 +5748,24 @@
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" s="21">
         <v>-1.6109690000000001</v>
@@ -5786,7 +5785,7 @@
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="20">
         <v>0.53407510000000002</v>
@@ -5806,7 +5805,7 @@
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="20">
         <v>0.71852899999999997</v>
@@ -5826,7 +5825,7 @@
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" s="20">
         <v>0.65963430000000001</v>
@@ -5846,7 +5845,7 @@
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="20">
         <v>3.3472799999999997E-2</v>
@@ -5866,7 +5865,7 @@
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B8" s="20">
         <v>1.11576E-2</v>
@@ -5886,7 +5885,7 @@
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B9" s="20">
         <v>0.50903609999999999</v>
@@ -5906,7 +5905,7 @@
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" s="20">
         <v>0.43028490000000003</v>
@@ -5926,7 +5925,7 @@
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B11" s="20">
         <v>0.22841230000000001</v>
@@ -5946,7 +5945,7 @@
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B12" s="20">
         <v>0.5823699</v>
@@ -5966,7 +5965,7 @@
     </row>
     <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="20">
         <v>0.70664740000000004</v>
@@ -5998,7 +5997,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:H21"/>
+      <selection sqref="A1:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6032,25 +6031,25 @@
     </row>
     <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -6549,7 +6548,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5">
         <f>SUM(B3:B21)</f>
@@ -6594,7 +6593,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6628,22 +6627,22 @@
     <row r="2" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6654,19 +6653,19 @@
         <v>72</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D3" s="6">
         <v>73</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6677,19 +6676,19 @@
         <v>197</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="6">
         <v>59</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6700,19 +6699,19 @@
         <v>152</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="6">
         <v>137</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6723,19 +6722,19 @@
         <v>40</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6">
         <v>167</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6746,19 +6745,19 @@
         <v>68</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D7" s="6">
         <v>89</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6769,19 +6768,19 @@
         <v>127</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D8" s="6">
         <v>118</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6792,19 +6791,19 @@
         <v>90</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9" s="6">
         <v>36</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6815,19 +6814,19 @@
         <v>130</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D10" s="10">
         <v>82</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6838,19 +6837,19 @@
         <v>61</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D11" s="6">
         <v>63</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6861,19 +6860,19 @@
         <v>114</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6">
         <v>31</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6884,19 +6883,19 @@
         <v>66</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D13" s="6">
         <v>97</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6907,19 +6906,19 @@
         <v>70</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D14" s="6">
         <v>121</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6930,19 +6929,19 @@
         <v>84</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D15" s="6">
         <v>134</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6953,19 +6952,19 @@
         <v>75</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D16" s="6">
         <v>164</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6976,19 +6975,19 @@
         <v>89</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D17" s="6">
         <v>129</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -6999,19 +6998,19 @@
         <v>66</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" s="6">
         <v>24</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -7022,19 +7021,19 @@
         <v>64</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D19" s="6">
         <v>190</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -7045,19 +7044,19 @@
         <v>60</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20" s="10">
         <v>88</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -7068,19 +7067,19 @@
         <v>113</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D21" s="6">
         <v>289</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -7096,8 +7095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F20955-0D28-BF41-ABD5-938E45A899BD}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7125,16 +7124,16 @@
     <row r="2" spans="1:5" ht="40" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="14" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7142,16 +7141,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>146</v>
+        <v>342</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>147</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7159,16 +7158,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>149</v>
+        <v>344</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>151</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7176,16 +7175,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>153</v>
+        <v>346</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7193,16 +7192,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>157</v>
+        <v>347</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7210,16 +7209,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7227,16 +7226,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>164</v>
+        <v>348</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7244,16 +7243,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7261,16 +7260,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>171</v>
+        <v>349</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7278,16 +7277,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>174</v>
+        <v>350</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7295,16 +7294,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>177</v>
+        <v>351</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7312,16 +7311,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>182</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7329,16 +7328,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>183</v>
+        <v>353</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7346,16 +7345,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>187</v>
+        <v>354</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>165</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7363,16 +7362,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>189</v>
+        <v>356</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7380,16 +7379,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>193</v>
+        <v>357</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7397,16 +7396,16 @@
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>196</v>
+        <v>358</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>198</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7414,16 +7413,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>200</v>
+        <v>360</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7431,16 +7430,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>203</v>
+        <v>361</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>205</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -7448,16 +7447,16 @@
         <v>18</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>207</v>
+        <v>363</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>118</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -7473,8 +7472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCB5F47-D317-AD4D-B9CB-3E22E29A0FD5}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F40" sqref="A1:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7503,39 +7502,39 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
-        <v>281</v>
-      </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="43"/>
+      <c r="B2" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="44"/>
       <c r="F2" s="42" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="22" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="44" t="s">
-        <v>279</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>279</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>284</v>
+      <c r="B3" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -7545,267 +7544,267 @@
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="29"/>
@@ -7815,207 +7814,207 @@
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="B29" s="36"/>
       <c r="C29" s="37"/>
@@ -8025,202 +8024,202 @@
     </row>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>